<commit_message>
Excel Dateien + Codekürzung
</commit_message>
<xml_diff>
--- a/Zeitmessung.xlsx
+++ b/Zeitmessung.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rickman\Documents\GitHub\Labrotation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3485AE71-ABC6-4EFA-8D47-C63381FDA957}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6753E50-E0DE-43AC-835B-687FBCA1BA02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{AB8AABE9-CED7-46F8-B858-5E8342E0FB0E}"/>
   </bookViews>
   <sheets>
     <sheet name="entropy.exe" sheetId="2" r:id="rId1"/>
     <sheet name="Biotite" sheetId="1" r:id="rId2"/>
+    <sheet name="both (sec)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>Länge (#AS)</t>
   </si>
@@ -88,12 +89,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -162,8 +164,159 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Laufzeit in Abhängigkeit von der Sequenzanzahl</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>entropy.exe!$B$2:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6500</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9500</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>entropy.exe!$D$2:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>236.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>316</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>398</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>479.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>559</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>640.70000000000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>720.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>799.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>881.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>965</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1040</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1122.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1208.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1286.0999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1363</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1444.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1526.6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1612</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1687.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A12B-432D-BB33-05EAD2805EB8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>Laufzeit in Abhängigkeit von der Sequenzanzahl</c:v>
           </c:tx>
@@ -333,7 +486,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-45F4-4634-A86A-0E8BD3ED932E}"/>
+              <c16:uniqueId val="{00000002-A12B-432D-BB33-05EAD2805EB8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -405,26 +558,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -524,26 +657,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -586,40 +699,12 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
   </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="lt1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -852,7 +937,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>10.85846601999998</c:v>
+                  <c:v>10.52569533999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>20.796041429999988</c:v>
@@ -861,55 +946,55 @@
                   <c:v>31.026360579999988</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41.155363899999998</c:v>
+                  <c:v>41.52296292999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>51.850572100000001</c:v>
+                  <c:v>51.72020774999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>61.606518600000001</c:v>
+                  <c:v>61.656381199999942</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>72.601781700000004</c:v>
+                  <c:v>71.976089539999975</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>82.634366099999994</c:v>
+                  <c:v>82.541414519999989</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>92.2457335</c:v>
+                  <c:v>93.164444459999956</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>106.0857037</c:v>
+                  <c:v>105.0186979299995</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>114.439594599999</c:v>
+                  <c:v>115.1004818599996</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>126.0719445</c:v>
+                  <c:v>125.3284759299997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>136.4052197</c:v>
+                  <c:v>135.28527714999981</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>145.5090534</c:v>
+                  <c:v>144.73433275999952</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>154.36748309999999</c:v>
+                  <c:v>154.32156652999981</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>162.3454418</c:v>
+                  <c:v>164.83060881999938</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>174.5796465</c:v>
+                  <c:v>174.4835180499995</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>184.3960515</c:v>
+                  <c:v>184.96870957999971</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>198.34530519999899</c:v>
+                  <c:v>197.21689612999961</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>208.3051882</c:v>
+                  <c:v>207.3877047499997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1232,6 +1317,883 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Laufzeiten</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>entropy.exe</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'both (sec)'!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6500</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9500</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'both (sec)'!$C$2:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.155</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.23619999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.316</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.39800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4793</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55900000000000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.64070000000000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7208</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79930000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.88190000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.96499999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>1.04</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.1223000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.2085000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.2861</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.363</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.4445000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.5266</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.6120000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.6871</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4B79-4AA9-A400-CA1B83859D93}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>biotite</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'both (sec)'!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6500</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9500</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'both (sec)'!$D$2:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>10.52569533999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.796041429999988</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.026360579999988</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41.52296292999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>51.72020774999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>61.656381199999942</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>71.976089539999975</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>82.541414519999989</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>93.164444459999956</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>105.0186979299995</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>115.1004818599996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>125.3284759299997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>135.28527714999981</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>144.73433275999952</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>154.32156652999981</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>164.83060881999938</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>174.4835180499995</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>184.96870957999971</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>197.21689612999961</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>207.3877047499997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4B79-4AA9-A400-CA1B83859D93}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="563583104"/>
+        <c:axId val="563586016"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="563583104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1200"/>
+                  <a:t>Anzahl der Sequenzen</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="563586016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="563586016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="210"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1200"/>
+                  <a:t>Zeit in</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1200" baseline="0"/>
+                  <a:t> Sekunden</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="563583104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1313,7 +2275,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1324,7 +2286,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="all"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -1340,25 +2302,25 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="bg1"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
@@ -1370,7 +2332,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -1378,11 +2340,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -1414,45 +2376,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="22225" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1464,26 +2416,22 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -1513,13 +2461,15 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1529,7 +2479,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1538,13 +2488,14 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1553,16 +2504,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -1571,10 +2523,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
@@ -1590,15 +2542,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1617,16 +2575,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -1635,16 +2594,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -1653,16 +2613,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -1683,7 +2644,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -1691,7 +2652,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -1704,17 +2665,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1722,10 +2672,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -1746,7 +2696,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1755,13 +2705,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1775,26 +2726,27 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="800" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1811,9 +2763,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1826,8 +2778,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2352,16 +3310,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>14286</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>14286</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4761</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2393,16 +3351,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>452437</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>642935</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>71436</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>452437</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>542924</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2410,6 +3368,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB9804CA-5D7A-4CB7-9AA6-3E24F4370A8C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BFF801F-5CF2-4DE2-A650-7C6A10761C82}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2729,8 +3728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F6BE54-4D76-41C4-A0E6-70103CACD823}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="P39" sqref="P39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3661,10 +4660,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04E3B570-B746-47C3-A5FA-F08E6D2C8A72}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3700,7 +4699,7 @@
       </c>
       <c r="D2" s="3">
         <f>AVERAGE(F2:O2)</f>
-        <v>10.85846601999998</v>
+        <v>10.52569533999997</v>
       </c>
       <c r="F2" s="1">
         <v>10.8877468</v>
@@ -3724,13 +4723,13 @@
         <v>10.5543017</v>
       </c>
       <c r="M2" s="1">
-        <v>11.3667192</v>
+        <v>10.356929399999901</v>
       </c>
       <c r="N2" s="1">
-        <v>11.4757649999999</v>
+        <v>10.201438099999899</v>
       </c>
       <c r="O2" s="1">
-        <v>11.3480238</v>
+        <v>10.304433700000001</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -3747,34 +4746,34 @@
         <f>AVERAGE(F3:O3)</f>
         <v>20.796041429999988</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="1">
         <v>20.935245099999999</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="1">
         <v>20.939360300000001</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="1">
         <v>20.859393699999998</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="1">
         <v>20.612740500000001</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="1">
         <v>20.718197399999902</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="1">
         <v>20.668050999999998</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="1">
         <v>20.9279726</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M3" s="1">
         <v>20.603787400000002</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N3" s="1">
         <v>20.814909400000001</v>
       </c>
-      <c r="O3" s="4">
+      <c r="O3" s="1">
         <v>20.880756900000002</v>
       </c>
     </row>
@@ -3792,34 +4791,34 @@
         <f t="shared" ref="D4:D21" si="0">AVERAGE(F4:O4)</f>
         <v>31.026360579999988</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="1">
         <v>30.870413899999999</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="1">
         <v>30.9684101</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="1">
         <v>30.749225599999999</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="1">
         <v>31.048568</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="1">
         <v>30.915784799999901</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="1">
         <v>31.116505</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="1">
         <v>31.9079321</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="1">
         <v>30.5013215</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="1">
         <v>31.0846296</v>
       </c>
-      <c r="O4" s="4">
+      <c r="O4" s="1">
         <v>31.1008152</v>
       </c>
     </row>
@@ -3835,20 +4834,38 @@
       </c>
       <c r="D5" s="3">
         <f t="shared" si="0"/>
-        <v>41.155363899999998</v>
-      </c>
-      <c r="F5" s="4">
-        <v>41.155363899999998</v>
-      </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
+        <v>41.52296292999997</v>
+      </c>
+      <c r="F5" s="1">
+        <v>42.117737099999999</v>
+      </c>
+      <c r="G5" s="1">
+        <v>42.469170400000003</v>
+      </c>
+      <c r="H5" s="1">
+        <v>41.783825399999998</v>
+      </c>
+      <c r="I5" s="1">
+        <v>41.144616699999901</v>
+      </c>
+      <c r="J5" s="1">
+        <v>41.006194899999997</v>
+      </c>
+      <c r="K5" s="1">
+        <v>41.329165600000003</v>
+      </c>
+      <c r="L5" s="1">
+        <v>41.502857199999902</v>
+      </c>
+      <c r="M5" s="1">
+        <v>41.247342600000003</v>
+      </c>
+      <c r="N5" s="1">
+        <v>41.405453700000002</v>
+      </c>
+      <c r="O5" s="1">
+        <v>41.223265699999899</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -3862,20 +4879,38 @@
       </c>
       <c r="D6" s="3">
         <f t="shared" si="0"/>
-        <v>51.850572100000001</v>
-      </c>
-      <c r="F6" s="4">
-        <v>51.850572100000001</v>
-      </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
+        <v>51.72020774999995</v>
+      </c>
+      <c r="F6" s="1">
+        <v>51.482221600000003</v>
+      </c>
+      <c r="G6" s="1">
+        <v>51.389327700000003</v>
+      </c>
+      <c r="H6" s="1">
+        <v>51.217257799999999</v>
+      </c>
+      <c r="I6" s="1">
+        <v>51.313749799999897</v>
+      </c>
+      <c r="J6" s="1">
+        <v>51.307070599999903</v>
+      </c>
+      <c r="K6" s="1">
+        <v>52.063825600000001</v>
+      </c>
+      <c r="L6" s="1">
+        <v>53.1022015</v>
+      </c>
+      <c r="M6" s="1">
+        <v>52.137505299999901</v>
+      </c>
+      <c r="N6" s="1">
+        <v>52.077739299999898</v>
+      </c>
+      <c r="O6" s="1">
+        <v>51.111178299999999</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -3889,20 +4924,38 @@
       </c>
       <c r="D7" s="3">
         <f t="shared" si="0"/>
-        <v>61.606518600000001</v>
-      </c>
-      <c r="F7" s="4">
-        <v>61.606518600000001</v>
-      </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
+        <v>61.656381199999942</v>
+      </c>
+      <c r="F7" s="1">
+        <v>61.423268100000001</v>
+      </c>
+      <c r="G7" s="1">
+        <v>61.269092299999897</v>
+      </c>
+      <c r="H7" s="1">
+        <v>62.822044599999998</v>
+      </c>
+      <c r="I7" s="1">
+        <v>61.173417899999997</v>
+      </c>
+      <c r="J7" s="1">
+        <v>62.625689099999903</v>
+      </c>
+      <c r="K7" s="1">
+        <v>61.024770899999901</v>
+      </c>
+      <c r="L7" s="1">
+        <v>61.7606877999999</v>
+      </c>
+      <c r="M7" s="1">
+        <v>61.0207257</v>
+      </c>
+      <c r="N7" s="1">
+        <v>62.0560104999999</v>
+      </c>
+      <c r="O7" s="1">
+        <v>61.388105099999898</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -3916,20 +4969,38 @@
       </c>
       <c r="D8" s="3">
         <f t="shared" si="0"/>
-        <v>72.601781700000004</v>
-      </c>
-      <c r="F8" s="4">
-        <v>72.601781700000004</v>
-      </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
+        <v>71.976089539999975</v>
+      </c>
+      <c r="F8" s="1">
+        <v>72.314297400000001</v>
+      </c>
+      <c r="G8" s="1">
+        <v>71.767113100000003</v>
+      </c>
+      <c r="H8" s="1">
+        <v>72.361094600000001</v>
+      </c>
+      <c r="I8" s="1">
+        <v>71.688007900000002</v>
+      </c>
+      <c r="J8" s="1">
+        <v>71.896290399999998</v>
+      </c>
+      <c r="K8" s="1">
+        <v>72.1038633</v>
+      </c>
+      <c r="L8" s="1">
+        <v>71.6916078</v>
+      </c>
+      <c r="M8" s="1">
+        <v>71.758812999999904</v>
+      </c>
+      <c r="N8" s="1">
+        <v>71.851796699999994</v>
+      </c>
+      <c r="O8" s="1">
+        <v>72.328011199999906</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -3943,20 +5014,38 @@
       </c>
       <c r="D9" s="3">
         <f t="shared" si="0"/>
-        <v>82.634366099999994</v>
-      </c>
-      <c r="F9" s="4">
-        <v>82.634366099999994</v>
-      </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
+        <v>82.541414519999989</v>
+      </c>
+      <c r="F9" s="1">
+        <v>82.518996299999998</v>
+      </c>
+      <c r="G9" s="1">
+        <v>81.813609999999997</v>
+      </c>
+      <c r="H9" s="1">
+        <v>82.860361499999996</v>
+      </c>
+      <c r="I9" s="1">
+        <v>82.011161799999897</v>
+      </c>
+      <c r="J9" s="1">
+        <v>83.018105599999998</v>
+      </c>
+      <c r="K9" s="1">
+        <v>82.237762500000002</v>
+      </c>
+      <c r="L9" s="1">
+        <v>81.802251799999993</v>
+      </c>
+      <c r="M9" s="1">
+        <v>82.787583999999995</v>
+      </c>
+      <c r="N9" s="1">
+        <v>82.034547799999999</v>
+      </c>
+      <c r="O9" s="1">
+        <v>84.329763899999904</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -3970,20 +5059,38 @@
       </c>
       <c r="D10" s="3">
         <f t="shared" si="0"/>
-        <v>92.2457335</v>
-      </c>
-      <c r="F10" s="4">
-        <v>92.2457335</v>
-      </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
+        <v>93.164444459999956</v>
+      </c>
+      <c r="F10" s="1">
+        <v>92.302910699999998</v>
+      </c>
+      <c r="G10" s="1">
+        <v>93.293521100000007</v>
+      </c>
+      <c r="H10" s="1">
+        <v>92.448414200000002</v>
+      </c>
+      <c r="I10" s="1">
+        <v>93.361421899999897</v>
+      </c>
+      <c r="J10" s="1">
+        <v>92.563752499999893</v>
+      </c>
+      <c r="K10" s="1">
+        <v>92.753065300000003</v>
+      </c>
+      <c r="L10" s="1">
+        <v>94.816908799999894</v>
+      </c>
+      <c r="M10" s="1">
+        <v>93.571773199999896</v>
+      </c>
+      <c r="N10" s="1">
+        <v>93.604004599999996</v>
+      </c>
+      <c r="O10" s="1">
+        <v>92.928672300000002</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -3997,20 +5104,38 @@
       </c>
       <c r="D11" s="3">
         <f t="shared" si="0"/>
-        <v>106.0857037</v>
-      </c>
-      <c r="F11" s="4">
-        <v>106.0857037</v>
-      </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
+        <v>105.0186979299995</v>
+      </c>
+      <c r="F11" s="1">
+        <v>104.0678357</v>
+      </c>
+      <c r="G11" s="1">
+        <v>102.618907499999</v>
+      </c>
+      <c r="H11" s="1">
+        <v>103.068999599999</v>
+      </c>
+      <c r="I11" s="1">
+        <v>103.019289299999</v>
+      </c>
+      <c r="J11" s="1">
+        <v>103.8696253</v>
+      </c>
+      <c r="K11" s="1">
+        <v>104.113175999999</v>
+      </c>
+      <c r="L11" s="1">
+        <v>116.90291980000001</v>
+      </c>
+      <c r="M11" s="1">
+        <v>106.137821</v>
+      </c>
+      <c r="N11" s="1">
+        <v>103.641628999999</v>
+      </c>
+      <c r="O11" s="1">
+        <v>102.74677610000001</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -4024,20 +5149,38 @@
       </c>
       <c r="D12" s="3">
         <f t="shared" si="0"/>
-        <v>114.439594599999</v>
-      </c>
-      <c r="F12" s="4">
-        <v>114.439594599999</v>
-      </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
+        <v>115.1004818599996</v>
+      </c>
+      <c r="F12" s="1">
+        <v>114.690042499999</v>
+      </c>
+      <c r="G12" s="1">
+        <v>113.1779906</v>
+      </c>
+      <c r="H12" s="1">
+        <v>116.41662479999999</v>
+      </c>
+      <c r="I12" s="1">
+        <v>115.03432410000001</v>
+      </c>
+      <c r="J12" s="1">
+        <v>114.60771089999901</v>
+      </c>
+      <c r="K12" s="1">
+        <v>114.06785609999901</v>
+      </c>
+      <c r="L12" s="1">
+        <v>115.4694849</v>
+      </c>
+      <c r="M12" s="1">
+        <v>117.4224191</v>
+      </c>
+      <c r="N12" s="1">
+        <v>115.843318099999</v>
+      </c>
+      <c r="O12" s="1">
+        <v>114.2750475</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -4051,20 +5194,38 @@
       </c>
       <c r="D13" s="3">
         <f t="shared" si="0"/>
-        <v>126.0719445</v>
-      </c>
-      <c r="F13" s="4">
-        <v>126.0719445</v>
-      </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
+        <v>125.3284759299997</v>
+      </c>
+      <c r="F13" s="1">
+        <v>126.260521</v>
+      </c>
+      <c r="G13" s="1">
+        <v>125.052110499999</v>
+      </c>
+      <c r="H13" s="1">
+        <v>125.9408406</v>
+      </c>
+      <c r="I13" s="1">
+        <v>123.7565651</v>
+      </c>
+      <c r="J13" s="1">
+        <v>127.9164954</v>
+      </c>
+      <c r="K13" s="1">
+        <v>125.338205899999</v>
+      </c>
+      <c r="L13" s="1">
+        <v>123.788236999999</v>
+      </c>
+      <c r="M13" s="1">
+        <v>123.91959850000001</v>
+      </c>
+      <c r="N13" s="1">
+        <v>128.7648733</v>
+      </c>
+      <c r="O13" s="1">
+        <v>122.54731200000001</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -4078,20 +5239,38 @@
       </c>
       <c r="D14" s="3">
         <f t="shared" si="0"/>
-        <v>136.4052197</v>
-      </c>
-      <c r="F14" s="4">
-        <v>136.4052197</v>
-      </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
+        <v>135.28527714999981</v>
+      </c>
+      <c r="F14" s="1">
+        <v>134.1293948</v>
+      </c>
+      <c r="G14" s="1">
+        <v>135.287577</v>
+      </c>
+      <c r="H14" s="1">
+        <v>132.35785730000001</v>
+      </c>
+      <c r="I14" s="1">
+        <v>134.856996199999</v>
+      </c>
+      <c r="J14" s="1">
+        <v>137.759113299999</v>
+      </c>
+      <c r="K14" s="1">
+        <v>138.36552270000001</v>
+      </c>
+      <c r="L14" s="1">
+        <v>133.65924559999999</v>
+      </c>
+      <c r="M14" s="1">
+        <v>136.02181580000001</v>
+      </c>
+      <c r="N14" s="1">
+        <v>135.92277540000001</v>
+      </c>
+      <c r="O14" s="1">
+        <v>134.49247339999999</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -4105,20 +5284,38 @@
       </c>
       <c r="D15" s="3">
         <f t="shared" si="0"/>
-        <v>145.5090534</v>
-      </c>
-      <c r="F15" s="4">
-        <v>145.5090534</v>
-      </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
+        <v>144.73433275999952</v>
+      </c>
+      <c r="F15" s="1">
+        <v>144.75688160000001</v>
+      </c>
+      <c r="G15" s="1">
+        <v>144.65128759999999</v>
+      </c>
+      <c r="H15" s="1">
+        <v>144.73122649999999</v>
+      </c>
+      <c r="I15" s="1">
+        <v>144.82544199999899</v>
+      </c>
+      <c r="J15" s="1">
+        <v>145.596698099999</v>
+      </c>
+      <c r="K15" s="1">
+        <v>143.68717089999899</v>
+      </c>
+      <c r="L15" s="1">
+        <v>145.69156779999901</v>
+      </c>
+      <c r="M15" s="1">
+        <v>145.480311499999</v>
+      </c>
+      <c r="N15" s="1">
+        <v>144.28321460000001</v>
+      </c>
+      <c r="O15" s="1">
+        <v>143.63952699999999</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -4132,20 +5329,38 @@
       </c>
       <c r="D16" s="3">
         <f t="shared" si="0"/>
-        <v>154.36748309999999</v>
-      </c>
-      <c r="F16" s="4">
-        <v>154.36748309999999</v>
-      </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
+        <v>154.32156652999981</v>
+      </c>
+      <c r="F16" s="1">
+        <v>153.48882409999999</v>
+      </c>
+      <c r="G16" s="1">
+        <v>154.6486141</v>
+      </c>
+      <c r="H16" s="1">
+        <v>154.56733059999999</v>
+      </c>
+      <c r="I16" s="1">
+        <v>153.90287369999999</v>
+      </c>
+      <c r="J16" s="1">
+        <v>156.05684299999899</v>
+      </c>
+      <c r="K16" s="1">
+        <v>153.33663039999999</v>
+      </c>
+      <c r="L16" s="1">
+        <v>155.61961220000001</v>
+      </c>
+      <c r="M16" s="1">
+        <v>153.64180390000001</v>
+      </c>
+      <c r="N16" s="1">
+        <v>154.89340530000001</v>
+      </c>
+      <c r="O16" s="1">
+        <v>153.05972799999901</v>
+      </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -4159,20 +5374,38 @@
       </c>
       <c r="D17" s="3">
         <f t="shared" si="0"/>
-        <v>162.3454418</v>
-      </c>
-      <c r="F17" s="4">
-        <v>162.3454418</v>
-      </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
+        <v>164.83060881999938</v>
+      </c>
+      <c r="F17" s="1">
+        <v>168.2600042</v>
+      </c>
+      <c r="G17" s="1">
+        <v>163.39432009999899</v>
+      </c>
+      <c r="H17" s="1">
+        <v>167.880157099999</v>
+      </c>
+      <c r="I17" s="1">
+        <v>166.11469600000001</v>
+      </c>
+      <c r="J17" s="1">
+        <v>162.83537580000001</v>
+      </c>
+      <c r="K17" s="1">
+        <v>166.34116789999899</v>
+      </c>
+      <c r="L17" s="1">
+        <v>163.44616059999899</v>
+      </c>
+      <c r="M17" s="1">
+        <v>162.63678389999899</v>
+      </c>
+      <c r="N17" s="1">
+        <v>164.6629623</v>
+      </c>
+      <c r="O17" s="1">
+        <v>162.734460299999</v>
+      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -4186,20 +5419,38 @@
       </c>
       <c r="D18" s="3">
         <f t="shared" si="0"/>
-        <v>174.5796465</v>
-      </c>
-      <c r="F18" s="4">
-        <v>174.5796465</v>
-      </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
+        <v>174.4835180499995</v>
+      </c>
+      <c r="F18" s="1">
+        <v>176.01854159999999</v>
+      </c>
+      <c r="G18" s="1">
+        <v>173.7795844</v>
+      </c>
+      <c r="H18" s="1">
+        <v>175.5790628</v>
+      </c>
+      <c r="I18" s="1">
+        <v>174.72132739999901</v>
+      </c>
+      <c r="J18" s="1">
+        <v>173.98974899999899</v>
+      </c>
+      <c r="K18" s="1">
+        <v>173.50412689999899</v>
+      </c>
+      <c r="L18" s="1">
+        <v>174.902834799999</v>
+      </c>
+      <c r="M18" s="1">
+        <v>174.59463559999901</v>
+      </c>
+      <c r="N18" s="1">
+        <v>174.26288829999999</v>
+      </c>
+      <c r="O18" s="1">
+        <v>173.48242970000001</v>
+      </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -4213,20 +5464,38 @@
       </c>
       <c r="D19" s="3">
         <f t="shared" si="0"/>
-        <v>184.3960515</v>
-      </c>
-      <c r="F19" s="4">
-        <v>184.3960515</v>
-      </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
+        <v>184.96870957999971</v>
+      </c>
+      <c r="F19" s="1">
+        <v>185.17722119999999</v>
+      </c>
+      <c r="G19" s="1">
+        <v>182.233138</v>
+      </c>
+      <c r="H19" s="1">
+        <v>185.82078349999901</v>
+      </c>
+      <c r="I19" s="1">
+        <v>186.59893120000001</v>
+      </c>
+      <c r="J19" s="1">
+        <v>183.39989489999999</v>
+      </c>
+      <c r="K19" s="1">
+        <v>186.71083390000001</v>
+      </c>
+      <c r="L19" s="1">
+        <v>183.76842439999899</v>
+      </c>
+      <c r="M19" s="1">
+        <v>185.6023946</v>
+      </c>
+      <c r="N19" s="1">
+        <v>184.341125199999</v>
+      </c>
+      <c r="O19" s="1">
+        <v>186.0343489</v>
+      </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -4240,20 +5509,38 @@
       </c>
       <c r="D20" s="3">
         <f t="shared" si="0"/>
-        <v>198.34530519999899</v>
-      </c>
-      <c r="F20" s="4">
-        <v>198.34530519999899</v>
-      </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
+        <v>197.21689612999961</v>
+      </c>
+      <c r="F20" s="1">
+        <v>203.91530909999901</v>
+      </c>
+      <c r="G20" s="1">
+        <v>195.39266319999999</v>
+      </c>
+      <c r="H20" s="1">
+        <v>196.2458091</v>
+      </c>
+      <c r="I20" s="1">
+        <v>198.03388829999901</v>
+      </c>
+      <c r="J20" s="1">
+        <v>199.652172699999</v>
+      </c>
+      <c r="K20" s="1">
+        <v>197.69189689999999</v>
+      </c>
+      <c r="L20" s="1">
+        <v>193.91816009999999</v>
+      </c>
+      <c r="M20" s="1">
+        <v>195.49272210000001</v>
+      </c>
+      <c r="N20" s="1">
+        <v>197.6332132</v>
+      </c>
+      <c r="O20" s="1">
+        <v>194.193126599999</v>
+      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -4267,24 +5554,398 @@
       </c>
       <c r="D21" s="3">
         <f t="shared" si="0"/>
-        <v>208.3051882</v>
-      </c>
-      <c r="F21" s="4">
-        <v>208.3051882</v>
-      </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
+        <v>207.3877047499997</v>
+      </c>
+      <c r="F21" s="1">
+        <v>200.51303590000001</v>
+      </c>
+      <c r="G21" s="1">
+        <v>214.47224600000001</v>
+      </c>
+      <c r="H21" s="1">
+        <v>208.68908549999901</v>
+      </c>
+      <c r="I21" s="1">
+        <v>206.02662900000001</v>
+      </c>
+      <c r="J21" s="1">
+        <v>210.26463290000001</v>
+      </c>
+      <c r="K21" s="1">
+        <v>208.41266719999999</v>
+      </c>
+      <c r="L21" s="1">
+        <v>206.01530349999899</v>
+      </c>
+      <c r="M21" s="1">
+        <v>206.35052719999999</v>
+      </c>
+      <c r="N21" s="1">
+        <v>206.3491922</v>
+      </c>
+      <c r="O21" s="1">
+        <v>206.783728099999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="I27" s="5"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="I28" s="5"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="I29" s="5"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="I30" s="5"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="I31" s="5"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="I32" s="5"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="I33" s="5"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G37" s="5"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G39" s="5"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G40" s="5"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G41" s="5"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G42" s="5"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G44" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5AEBD55-0F0B-4BD6-88A2-7B76C5CFD389}">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>500</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.155</v>
+      </c>
+      <c r="D2" s="4">
+        <v>10.52569533999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1000</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.23619999999999999</v>
+      </c>
+      <c r="D3" s="4">
+        <v>20.796041429999988</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1500</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.316</v>
+      </c>
+      <c r="D4" s="4">
+        <v>31.026360579999988</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2000</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="D5" s="4">
+        <v>41.52296292999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2500</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.4793</v>
+      </c>
+      <c r="D6" s="4">
+        <v>51.72020774999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3000</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="D7" s="4">
+        <v>61.656381199999942</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3500</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.64070000000000005</v>
+      </c>
+      <c r="D8" s="4">
+        <v>71.976089539999975</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4000</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.7208</v>
+      </c>
+      <c r="D9" s="4">
+        <v>82.541414519999989</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4500</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.79930000000000001</v>
+      </c>
+      <c r="D10" s="4">
+        <v>93.164444459999956</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5000</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.88190000000000002</v>
+      </c>
+      <c r="D11" s="4">
+        <v>105.0186979299995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5500</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="D12" s="4">
+        <v>115.1004818599996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>6000</v>
+      </c>
+      <c r="C13">
+        <v>1.04</v>
+      </c>
+      <c r="D13" s="4">
+        <v>125.3284759299997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>6500</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1.1223000000000001</v>
+      </c>
+      <c r="D14" s="4">
+        <v>135.28527714999981</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>7000</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1.2085000000000001</v>
+      </c>
+      <c r="D15" s="4">
+        <v>144.73433275999952</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>7500</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1.2861</v>
+      </c>
+      <c r="D16" s="4">
+        <v>154.32156652999981</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>8000</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1.363</v>
+      </c>
+      <c r="D17" s="4">
+        <v>164.83060881999938</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>8500</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1.4445000000000001</v>
+      </c>
+      <c r="D18" s="4">
+        <v>174.4835180499995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>9000</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1.5266</v>
+      </c>
+      <c r="D19" s="4">
+        <v>184.96870957999971</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>9500</v>
+      </c>
+      <c r="C20" s="4">
+        <v>1.6120000000000001</v>
+      </c>
+      <c r="D20" s="4">
+        <v>197.21689612999961</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>10000</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1.6871</v>
+      </c>
+      <c r="D21" s="4">
+        <v>207.3877047499997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>